<commit_message>
Need to commit in order to pull
</commit_message>
<xml_diff>
--- a/Documentation/Product backlog+Sprint1.xlsx
+++ b/Documentation/Product backlog+Sprint1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11820" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="19155" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
   <si>
     <t>Developers</t>
   </si>
@@ -206,7 +206,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +237,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="3" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -258,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -267,6 +296,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,11 +601,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J89"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K73" sqref="K73"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +664,7 @@
         <v>30</v>
       </c>
       <c r="D2">
-        <f>C2-(SUMIF(F2:F85,"=JB",G2:G85))</f>
+        <f>C2-(SUMIF(F2:F89,"=JB",G2:G89))</f>
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -655,7 +688,7 @@
         <v>30</v>
       </c>
       <c r="D3">
-        <f ca="1">C3-(SUMIF(F8:F85,"=RO",G8:G83))</f>
+        <f ca="1">C3-(SUMIF(F8:F89,"=RO",G8:G87))</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -665,11 +698,11 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3">
         <f>G3-H3</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="4"/>
     </row>
@@ -684,8 +717,8 @@
         <v>30</v>
       </c>
       <c r="D4">
-        <f ca="1">C4-(SUMIF(F3:F85,"=CS",G3:G83))</f>
-        <v>0</v>
+        <f ca="1">C4-(SUMIF(F3:F89,"=CS",G3:G87))</f>
+        <v>-8</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -694,11 +727,11 @@
         <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I67" si="0">G4-H4</f>
-        <v>1</v>
+        <f t="shared" ref="I4:I11" si="0">G4-H4</f>
+        <v>0</v>
       </c>
       <c r="J4" s="4"/>
     </row>
@@ -713,8 +746,8 @@
         <v>30</v>
       </c>
       <c r="D5">
-        <f ca="1">C5-(SUMIF(F18:F85,"=IL",G18:G83))</f>
-        <v>0</v>
+        <f ca="1">C5-(SUMIF(F20:F89,"=IL",G20:G87))</f>
+        <v>-3</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
@@ -739,11 +772,11 @@
         <v>1</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="4"/>
     </row>
@@ -780,491 +813,521 @@
         <v>3</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-2</v>
       </c>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="7">
+        <v>3</v>
+      </c>
+      <c r="H10" s="7">
+        <v>5</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="7">
+        <v>3</v>
+      </c>
+      <c r="H11" s="7">
+        <v>5</v>
+      </c>
+      <c r="I11" s="7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F12" t="s">
         <v>6</v>
       </c>
-      <c r="G10">
+      <c r="G12">
         <v>2</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <f>G12-H12</f>
+        <v>-1</v>
+      </c>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14">
+        <f>G14-H14</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>G15-H15</f>
+        <v>5</v>
+      </c>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="7">
+        <v>5</v>
+      </c>
+      <c r="H16" s="7">
+        <v>5</v>
+      </c>
+      <c r="I16" s="7">
+        <f>G16-H16</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17">
+        <f>G17-H17</f>
+        <v>0</v>
+      </c>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18">
         <v>2</v>
       </c>
-      <c r="J10" s="4"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J11" s="4"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J13" s="4"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="4"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" t="s">
-        <v>7</v>
-      </c>
-      <c r="G16">
+      <c r="H18">
         <v>2</v>
       </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J16" s="4"/>
-    </row>
-    <row r="17" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J17" s="4"/>
-    </row>
-    <row r="18" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E18" s="1" t="s">
+      <c r="I18">
+        <f>G18-H18</f>
+        <v>0</v>
+      </c>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J18" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G19">
-        <v>0.5</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-      <c r="J19" s="4"/>
-    </row>
-    <row r="20" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E20" t="s">
-        <v>43</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
       </c>
-      <c r="G20">
-        <v>3.5</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
       <c r="I20">
-        <f t="shared" si="0"/>
-        <v>3.5</v>
-      </c>
-      <c r="J20" s="4"/>
+        <f>G20-H20</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F21" t="s">
         <v>8</v>
       </c>
       <c r="G21">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G21-H21</f>
+        <v>0.5</v>
       </c>
       <c r="J21" s="4"/>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F22" t="s">
         <v>8</v>
       </c>
       <c r="G22">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="H22">
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G22-H22</f>
+        <v>3.5</v>
       </c>
       <c r="J22" s="4"/>
     </row>
     <row r="23" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>G23-H23</f>
+        <v>3</v>
       </c>
       <c r="J23" s="4"/>
     </row>
     <row r="24" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F24" t="s">
         <v>8</v>
       </c>
       <c r="G24">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>G24-H24</f>
+        <v>3</v>
       </c>
       <c r="J24" s="4"/>
     </row>
     <row r="25" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F25" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G25-H25</f>
+        <v>2</v>
       </c>
       <c r="J25" s="4"/>
     </row>
     <row r="26" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F26" t="s">
         <v>8</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G26-H26</f>
+        <v>5</v>
       </c>
       <c r="J26" s="4"/>
     </row>
     <row r="27" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <f>G27-H27</f>
+        <v>1</v>
+      </c>
       <c r="J27" s="4"/>
     </row>
     <row r="28" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <f>G28-H28</f>
+        <v>1</v>
+      </c>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F28" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J28" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" t="s">
-        <v>7</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>0</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J29" s="4"/>
-    </row>
-    <row r="30" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
-        <v>47</v>
-      </c>
       <c r="F30" t="s">
-        <v>6</v>
-      </c>
-      <c r="G30">
-        <v>1</v>
-      </c>
-      <c r="H30">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J30" s="4"/>
+        <f>G30-H30</f>
+        <v>0</v>
+      </c>
+      <c r="J30" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="31" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
+        <v>41</v>
+      </c>
+      <c r="F31" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31">
+        <f>G31-H31</f>
+        <v>2</v>
+      </c>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" s="7">
+        <v>2</v>
+      </c>
+      <c r="H32" s="7">
+        <v>3</v>
+      </c>
+      <c r="I32" s="7">
+        <f>G32-H32</f>
+        <v>-1</v>
+      </c>
+      <c r="J32" s="7"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
         <v>47</v>
       </c>
-      <c r="F31" t="s">
-        <v>7</v>
-      </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J31" s="4"/>
-    </row>
-    <row r="32" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J32" s="4"/>
-    </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E33" s="1" t="s">
-        <v>20</v>
+      <c r="F33" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="4">
-        <v>5</v>
-      </c>
+        <f>G33-H33</f>
+        <v>1</v>
+      </c>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G34">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>G34-H34</f>
+        <v>1</v>
       </c>
       <c r="J34" s="4"/>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>45</v>
-      </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35">
-        <v>3</v>
-      </c>
-      <c r="H35">
-        <v>0</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J35" s="4"/>
-    </row>
     <row r="36" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>45</v>
-      </c>
-      <c r="F36" t="s">
-        <v>7</v>
-      </c>
-      <c r="G36">
-        <v>2</v>
-      </c>
-      <c r="H36">
-        <v>0</v>
+      <c r="E36" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="I36">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J36" s="4"/>
+        <f>G36-H36</f>
+        <v>0</v>
+      </c>
+      <c r="J36" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
       </c>
       <c r="G37">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>G37-H37</f>
+        <v>2</v>
       </c>
       <c r="J37" s="4"/>
     </row>
     <row r="38" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G38-H38</f>
+        <v>3</v>
       </c>
       <c r="J38" s="4"/>
     </row>
     <row r="39" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
+        <v>45</v>
+      </c>
+      <c r="F39" t="s">
+        <v>7</v>
+      </c>
+      <c r="G39">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f>G39-H39</f>
+        <v>2</v>
+      </c>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>5</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <f>G40-H40</f>
+        <v>5</v>
+      </c>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E41" t="s">
         <v>47</v>
       </c>
-      <c r="F39" t="s">
-        <v>8</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J40" s="4"/>
-    </row>
-    <row r="41" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E41" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="F41" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
       </c>
       <c r="I41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J41" s="4">
-        <v>7</v>
-      </c>
+        <f>G41-H41</f>
+        <v>1</v>
+      </c>
+      <c r="J41" s="4"/>
     </row>
     <row r="42" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -1273,52 +1336,32 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <f t="shared" si="0"/>
+        <f>G42-H42</f>
         <v>1</v>
       </c>
       <c r="J42" s="4"/>
     </row>
     <row r="43" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
-        <v>52</v>
-      </c>
-      <c r="F43" t="s">
-        <v>7</v>
-      </c>
-      <c r="G43">
-        <v>0.5</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
       <c r="J43" s="4"/>
     </row>
     <row r="44" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
-        <v>47</v>
+      <c r="E44" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="F44" t="s">
-        <v>6</v>
-      </c>
-      <c r="G44">
-        <v>1</v>
-      </c>
-      <c r="H44">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="J44" s="4"/>
+        <f>G44-H44</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="45" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F45" t="s">
         <v>7</v>
@@ -1330,299 +1373,310 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
+        <f>G45-H45</f>
         <v>1</v>
       </c>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J46" s="4"/>
+      <c r="E46" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" t="s">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>3</v>
+      </c>
+      <c r="I46">
+        <f>G46-H46</f>
+        <v>-2</v>
+      </c>
+      <c r="J46" s="9"/>
     </row>
     <row r="47" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E47" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="I47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="4">
-        <v>8</v>
-      </c>
+      <c r="E47" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="H47" s="8">
+        <v>0</v>
+      </c>
+      <c r="I47" s="8">
+        <f>G47-H47</f>
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="4"/>
     </row>
     <row r="48" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F48" t="s">
         <v>6</v>
       </c>
       <c r="G48">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H48">
         <v>0</v>
       </c>
       <c r="I48">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>G48-H48</f>
+        <v>1</v>
       </c>
       <c r="J48" s="4"/>
     </row>
-    <row r="49" spans="5:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E49" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G49">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
       <c r="I49">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G49-H49</f>
+        <v>1</v>
       </c>
       <c r="J49" s="4"/>
     </row>
-    <row r="50" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" t="s">
-        <v>6</v>
-      </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
-        <v>0</v>
-      </c>
-      <c r="I50">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
+    <row r="50" spans="5:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J50" s="4"/>
     </row>
     <row r="51" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
-        <v>45</v>
-      </c>
-      <c r="F51" t="s">
-        <v>7</v>
-      </c>
-      <c r="G51">
-        <v>2</v>
-      </c>
-      <c r="H51">
-        <v>0</v>
+      <c r="E51" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="I51">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="J51" s="4"/>
+        <f>G51-H51</f>
+        <v>0</v>
+      </c>
+      <c r="J51" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="52" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E52" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="F52" t="s">
         <v>6</v>
       </c>
       <c r="G52">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H52">
         <v>0</v>
       </c>
       <c r="I52">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G52-H52</f>
+        <v>4</v>
       </c>
       <c r="J52" s="4"/>
     </row>
     <row r="53" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E53" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F53" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H53">
         <v>0</v>
       </c>
       <c r="I53">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G53-H53</f>
+        <v>3</v>
       </c>
       <c r="J53" s="4"/>
     </row>
     <row r="54" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>45</v>
+      </c>
+      <c r="F54" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
       <c r="I54">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>G54-H54</f>
+        <v>2</v>
       </c>
       <c r="J54" s="4"/>
     </row>
     <row r="55" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E55" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J55" s="4">
-        <v>8</v>
-      </c>
+      <c r="E55" t="s">
+        <v>45</v>
+      </c>
+      <c r="F55" t="s">
+        <v>7</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f>G55-H55</f>
+        <v>2</v>
+      </c>
+      <c r="J55" s="4"/>
     </row>
     <row r="56" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="F56" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G56">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H56">
         <v>0</v>
       </c>
       <c r="I56">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>G56-H56</f>
+        <v>3</v>
       </c>
       <c r="J56" s="4"/>
     </row>
     <row r="57" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="F57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G57">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H57">
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G57-H57</f>
+        <v>1</v>
       </c>
       <c r="J57" s="4"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E58" t="s">
-        <v>45</v>
-      </c>
-      <c r="F58" t="s">
-        <v>9</v>
-      </c>
-      <c r="G58">
-        <v>3</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
       <c r="I58">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G58-H58</f>
+        <v>0</v>
       </c>
       <c r="J58" s="4"/>
     </row>
     <row r="59" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
-        <v>45</v>
-      </c>
-      <c r="F59" t="s">
-        <v>7</v>
-      </c>
-      <c r="G59">
-        <v>3</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-      <c r="I59">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J59" s="4"/>
+      <c r="E59" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J59" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="60" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E60" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="F60" t="s">
         <v>9</v>
       </c>
       <c r="G60">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H60">
         <v>0</v>
       </c>
       <c r="I60">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G60-H60</f>
+        <v>4</v>
       </c>
       <c r="J60" s="4"/>
     </row>
     <row r="61" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F61" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H61">
         <v>0</v>
       </c>
       <c r="I61">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G61-H61</f>
+        <v>3</v>
       </c>
       <c r="J61" s="4"/>
     </row>
     <row r="62" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F62" t="s">
         <v>9</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H62">
         <v>0</v>
       </c>
       <c r="I62">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>G62-H62</f>
+        <v>3</v>
       </c>
       <c r="J62" s="4"/>
     </row>
     <row r="63" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E63" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J63" s="4">
-        <v>8</v>
-      </c>
+      <c r="E63" t="s">
+        <v>45</v>
+      </c>
+      <c r="F63" t="s">
+        <v>7</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <f>G63-H63</f>
+        <v>3</v>
+      </c>
+      <c r="J63" s="4"/>
     </row>
     <row r="64" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E64" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="F64" t="s">
         <v>9</v>
@@ -1634,71 +1688,60 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <f t="shared" si="0"/>
+        <f>G64-H64</f>
         <v>3</v>
       </c>
       <c r="J64" s="4"/>
     </row>
     <row r="65" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E65" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F65" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G65">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H65">
         <v>0</v>
       </c>
       <c r="I65">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>G65-H65</f>
+        <v>1</v>
       </c>
       <c r="J65" s="4"/>
     </row>
     <row r="66" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E66" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F66" t="s">
         <v>9</v>
       </c>
       <c r="G66">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H66">
         <v>0</v>
       </c>
       <c r="I66">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>G66-H66</f>
+        <v>1</v>
       </c>
       <c r="J66" s="4"/>
     </row>
     <row r="67" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
-        <v>45</v>
-      </c>
-      <c r="F67" t="s">
-        <v>7</v>
-      </c>
-      <c r="G67">
-        <v>3</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-      <c r="I67">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="J67" s="4"/>
+      <c r="E67" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J67" s="4">
+        <v>8</v>
+      </c>
     </row>
     <row r="68" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E68" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="F68" t="s">
         <v>9</v>
@@ -1710,76 +1753,103 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <f t="shared" ref="I68:I82" si="1">G68-H68</f>
+        <f>G68-H68</f>
         <v>3</v>
       </c>
       <c r="J68" s="4"/>
     </row>
     <row r="69" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E69" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="F69" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H69">
         <v>0</v>
       </c>
       <c r="I69">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>G69-H69</f>
+        <v>5</v>
       </c>
       <c r="J69" s="4"/>
     </row>
     <row r="70" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E70" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F70" t="s">
         <v>9</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H70">
         <v>0</v>
       </c>
       <c r="I70">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f>G70-H70</f>
+        <v>3</v>
       </c>
       <c r="J70" s="4"/>
     </row>
     <row r="71" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E71" t="s">
+        <v>45</v>
+      </c>
+      <c r="F71" t="s">
+        <v>7</v>
+      </c>
+      <c r="G71">
+        <v>3</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <f>G71-H71</f>
+        <v>3</v>
+      </c>
       <c r="J71" s="4"/>
     </row>
     <row r="72" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E72" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J72" s="4">
-        <v>7</v>
-      </c>
+      <c r="E72" t="s">
+        <v>46</v>
+      </c>
+      <c r="F72" t="s">
+        <v>9</v>
+      </c>
+      <c r="G72">
+        <v>3</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <f t="shared" ref="I72:I74" si="1">G72-H72</f>
+        <v>3</v>
+      </c>
+      <c r="J72" s="4"/>
     </row>
     <row r="73" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E73" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F73" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G73">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="H73">
         <v>0</v>
       </c>
       <c r="I73">
-        <f>G73-H73</f>
-        <v>2.5</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="J73" s="4"/>
     </row>
@@ -1788,7 +1858,7 @@
         <v>47</v>
       </c>
       <c r="F74" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G74">
         <v>1</v>
@@ -1797,69 +1867,69 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <f>G74-H74</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J74" s="4"/>
     </row>
     <row r="75" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
-        <v>47</v>
-      </c>
-      <c r="F75" t="s">
-        <v>7</v>
-      </c>
-      <c r="G75">
-        <v>1</v>
-      </c>
-      <c r="I75">
-        <f>G75-H75</f>
-        <v>1</v>
-      </c>
       <c r="J75" s="4"/>
     </row>
     <row r="76" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J76" s="5"/>
+      <c r="E76" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J76" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="77" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E77" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J77" s="4">
-        <v>7</v>
-      </c>
+      <c r="E77" t="s">
+        <v>60</v>
+      </c>
+      <c r="F77" t="s">
+        <v>7</v>
+      </c>
+      <c r="G77">
+        <v>2.5</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77">
+        <f>G77-H77</f>
+        <v>2.5</v>
+      </c>
+      <c r="J77" s="4"/>
     </row>
     <row r="78" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E78" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F78" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H78">
         <v>0</v>
       </c>
       <c r="I78">
         <f>G78-H78</f>
-        <v>2</v>
-      </c>
-      <c r="J78" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="J78" s="4"/>
     </row>
     <row r="79" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E79" t="s">
         <v>47</v>
       </c>
       <c r="F79" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G79">
         <v>1</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
       </c>
       <c r="I79">
         <f>G79-H79</f>
@@ -1868,60 +1938,60 @@
       <c r="J79" s="4"/>
     </row>
     <row r="80" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E80" t="s">
-        <v>47</v>
-      </c>
-      <c r="F80" t="s">
-        <v>7</v>
-      </c>
-      <c r="G80">
-        <v>1</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-      <c r="I80">
-        <f>G80-H80</f>
-        <v>1</v>
-      </c>
-      <c r="J80" s="4"/>
+      <c r="J80" s="5"/>
     </row>
     <row r="81" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="J81" s="5"/>
+      <c r="E81" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J81" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="82" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E82" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J82" s="4">
-        <v>7</v>
-      </c>
+      <c r="E82" t="s">
+        <v>60</v>
+      </c>
+      <c r="F82" t="s">
+        <v>7</v>
+      </c>
+      <c r="G82">
+        <v>2</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82">
+        <f>G82-H82</f>
+        <v>2</v>
+      </c>
+      <c r="J82" s="5"/>
     </row>
     <row r="83" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E83" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="F83" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G83">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H83">
         <v>0</v>
       </c>
       <c r="I83">
         <f>G83-H83</f>
-        <v>3</v>
-      </c>
-      <c r="J83" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="J83" s="4"/>
     </row>
     <row r="84" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E84" t="s">
         <v>47</v>
       </c>
       <c r="F84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G84">
         <v>1</v>
@@ -1933,23 +2003,72 @@
         <f>G84-H84</f>
         <v>1</v>
       </c>
-      <c r="J84" s="5"/>
+      <c r="J84" s="4"/>
     </row>
     <row r="85" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
+      <c r="J85" s="5"/>
+    </row>
+    <row r="86" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E86" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J86" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>60</v>
+      </c>
+      <c r="F87" t="s">
+        <v>7</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+      <c r="I87">
+        <f>G87-H87</f>
+        <v>3</v>
+      </c>
+      <c r="J87" s="5"/>
+    </row>
+    <row r="88" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
         <v>47</v>
       </c>
-      <c r="F85" t="s">
-        <v>7</v>
-      </c>
-      <c r="G85">
-        <v>1</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-      <c r="I85">
-        <f>G85-H85</f>
+      <c r="F88" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88">
+        <v>1</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <f>G88-H88</f>
+        <v>1</v>
+      </c>
+      <c r="J88" s="5"/>
+    </row>
+    <row r="89" spans="5:10" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>47</v>
+      </c>
+      <c r="F89" t="s">
+        <v>7</v>
+      </c>
+      <c r="G89">
+        <v>1</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+      <c r="I89">
+        <f>G89-H89</f>
         <v>1</v>
       </c>
     </row>
@@ -1961,10 +2080,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2036,6 +2155,18 @@
       <c r="F8">
         <v>3</v>
       </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Product Backlog with some updates, still needs review
</commit_message>
<xml_diff>
--- a/Documentation/Product backlog+Sprint1.xlsx
+++ b/Documentation/Product backlog+Sprint1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="62">
   <si>
     <t>Developers</t>
   </si>
@@ -200,6 +200,9 @@
   </si>
   <si>
     <t xml:space="preserve">    Simple UI</t>
+  </si>
+  <si>
+    <t>Not needed</t>
   </si>
 </sst>
 </file>
@@ -604,8 +607,8 @@
   <dimension ref="A1:J89"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J90" sqref="J90"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J60" sqref="J60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,7 +968,7 @@
         <v>8</v>
       </c>
       <c r="I20">
-        <f>G20-H20</f>
+        <f t="shared" ref="I20:I28" si="1">G20-H20</f>
         <v>0</v>
       </c>
       <c r="J20" s="4">
@@ -973,23 +976,25 @@
       </c>
     </row>
     <row r="21" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E21" t="s">
+      <c r="E21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="5">
         <v>0.5</v>
       </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <f>G21-H21</f>
+      <c r="H21" s="5">
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="J21" s="4"/>
+      <c r="J21" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" spans="5:10" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
@@ -1002,11 +1007,11 @@
         <v>3.5</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I22">
-        <f>G22-H22</f>
-        <v>3.5</v>
+        <f t="shared" si="1"/>
+        <v>-1.5</v>
       </c>
       <c r="J22" s="4"/>
     </row>
@@ -1021,11 +1026,11 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I23">
-        <f>G23-H23</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>-1</v>
       </c>
       <c r="J23" s="4"/>
     </row>
@@ -1040,11 +1045,11 @@
         <v>3</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I24">
-        <f>G24-H24</f>
-        <v>3</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="J24" s="4"/>
     </row>
@@ -1062,7 +1067,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <f>G25-H25</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J25" s="4"/>
@@ -1081,7 +1086,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f>G26-H26</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="J26" s="4"/>
@@ -1100,7 +1105,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f>G27-H27</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J27" s="4"/>
@@ -1119,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f>G28-H28</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J28" s="4"/>
@@ -1220,7 +1225,7 @@
         <v>20</v>
       </c>
       <c r="I36">
-        <f>G36-H36</f>
+        <f t="shared" ref="I36:I42" si="2">G36-H36</f>
         <v>0</v>
       </c>
       <c r="J36" s="4">
@@ -1241,7 +1246,7 @@
         <v>0</v>
       </c>
       <c r="I37">
-        <f>G37-H37</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J37" s="4"/>
@@ -1260,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="I38">
-        <f>G38-H38</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J38" s="4"/>
@@ -1279,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="I39">
-        <f>G39-H39</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J39" s="4"/>
@@ -1298,7 +1303,7 @@
         <v>0</v>
       </c>
       <c r="I40">
-        <f>G40-H40</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J40" s="4"/>
@@ -1317,7 +1322,7 @@
         <v>0</v>
       </c>
       <c r="I41">
-        <f>G41-H41</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J41" s="4"/>
@@ -1336,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <f>G42-H42</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="J42" s="4"/>
@@ -1352,7 +1357,7 @@
         <v>7</v>
       </c>
       <c r="I44">
-        <f>G44-H44</f>
+        <f t="shared" ref="I44:I49" si="3">G44-H44</f>
         <v>0</v>
       </c>
       <c r="J44" s="4">
@@ -1373,26 +1378,26 @@
         <v>0</v>
       </c>
       <c r="I45">
-        <f>G45-H45</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J45" s="4"/>
     </row>
     <row r="46" spans="5:10" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
+      <c r="E46" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F46" t="s">
+      <c r="F46" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G46">
-        <v>1</v>
-      </c>
-      <c r="H46">
-        <v>3</v>
-      </c>
-      <c r="I46">
-        <f>G46-H46</f>
+      <c r="G46" s="7">
+        <v>1</v>
+      </c>
+      <c r="H46" s="7">
+        <v>3</v>
+      </c>
+      <c r="I46" s="7">
+        <f t="shared" si="3"/>
         <v>-2</v>
       </c>
       <c r="J46" s="9"/>
@@ -1411,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="8">
-        <f>G47-H47</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="J47" s="4"/>
@@ -1430,7 +1435,7 @@
         <v>0</v>
       </c>
       <c r="I48">
-        <f>G48-H48</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J48" s="4"/>
@@ -1449,7 +1454,7 @@
         <v>0</v>
       </c>
       <c r="I49">
-        <f>G49-H49</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J49" s="4"/>
@@ -1462,7 +1467,7 @@
         <v>22</v>
       </c>
       <c r="I51">
-        <f>G51-H51</f>
+        <f t="shared" ref="I51:I58" si="4">G51-H51</f>
         <v>0</v>
       </c>
       <c r="J51" s="4">
@@ -1480,11 +1485,11 @@
         <v>4</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I52">
-        <f>G52-H52</f>
-        <v>4</v>
+        <f t="shared" si="4"/>
+        <v>-1</v>
       </c>
       <c r="J52" s="4"/>
     </row>
@@ -1499,11 +1504,11 @@
         <v>3</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I53">
-        <f>G53-H53</f>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>-1</v>
       </c>
       <c r="J53" s="4"/>
     </row>
@@ -1518,11 +1523,11 @@
         <v>2</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I54">
-        <f>G54-H54</f>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
       <c r="J54" s="4"/>
     </row>
@@ -1540,7 +1545,7 @@
         <v>0</v>
       </c>
       <c r="I55">
-        <f>G55-H55</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="J55" s="4"/>
@@ -1559,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="I56">
-        <f>G56-H56</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="J56" s="4"/>
@@ -1578,14 +1583,14 @@
         <v>0</v>
       </c>
       <c r="I57">
-        <f>G57-H57</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="J57" s="4"/>
     </row>
     <row r="58" spans="5:10" x14ac:dyDescent="0.25">
       <c r="I58">
-        <f>G58-H58</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J58" s="4"/>
@@ -1612,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="I60">
-        <f>G60-H60</f>
+        <f t="shared" ref="I60:I66" si="5">G60-H60</f>
         <v>4</v>
       </c>
       <c r="J60" s="4"/>
@@ -1631,7 +1636,7 @@
         <v>0</v>
       </c>
       <c r="I61">
-        <f>G61-H61</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J61" s="4"/>
@@ -1650,7 +1655,7 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <f>G62-H62</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J62" s="4"/>
@@ -1669,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="I63">
-        <f>G63-H63</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J63" s="4"/>
@@ -1688,7 +1693,7 @@
         <v>0</v>
       </c>
       <c r="I64">
-        <f>G64-H64</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="J64" s="4"/>
@@ -1707,7 +1712,7 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <f>G65-H65</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J65" s="4"/>
@@ -1726,7 +1731,7 @@
         <v>0</v>
       </c>
       <c r="I66">
-        <f>G66-H66</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J66" s="4"/>
@@ -1829,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <f t="shared" ref="I72:I74" si="1">G72-H72</f>
+        <f t="shared" ref="I72:I74" si="6">G72-H72</f>
         <v>3</v>
       </c>
       <c r="J72" s="4"/>
@@ -1848,7 +1853,7 @@
         <v>0</v>
       </c>
       <c r="I73">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J73" s="4"/>
@@ -1867,7 +1872,7 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="J74" s="4"/>
@@ -1930,6 +1935,9 @@
       </c>
       <c r="G79">
         <v>1</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
       </c>
       <c r="I79">
         <f>G79-H79</f>

</xml_diff>

<commit_message>
Fixed account creation bug, modified contacts ui, account login working
</commit_message>
<xml_diff>
--- a/Documentation/Product backlog+Sprint1.xlsx
+++ b/Documentation/Product backlog+Sprint1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="69">
   <si>
     <t>Developers</t>
   </si>
@@ -218,13 +218,19 @@
   </si>
   <si>
     <t xml:space="preserve">Drag and Drop functionality </t>
+  </si>
+  <si>
+    <t>Add security to our database and REST calls</t>
+  </si>
+  <si>
+    <t>addition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +313,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -339,6 +353,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -352,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -375,6 +395,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1848,7 +1870,7 @@
         <v>0</v>
       </c>
       <c r="I68">
-        <f>G68-H68</f>
+        <f t="shared" ref="I68:I73" si="6">G68-H68</f>
         <v>3</v>
       </c>
       <c r="J68" s="4"/>
@@ -1867,7 +1889,7 @@
         <v>0</v>
       </c>
       <c r="I69">
-        <f>G69-H69</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="J69" s="4"/>
@@ -1886,7 +1908,7 @@
         <v>3</v>
       </c>
       <c r="I70" s="7">
-        <f>G70-H70</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J70" s="4"/>
@@ -1905,7 +1927,7 @@
         <v>5</v>
       </c>
       <c r="I71" s="7">
-        <f>G71-H71</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -1923,7 +1945,7 @@
         <v>3</v>
       </c>
       <c r="I72">
-        <f>G72-H72</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J72" s="4"/>
@@ -1942,7 +1964,7 @@
         <v>0</v>
       </c>
       <c r="I73" s="14">
-        <f>G73-H73</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="J73" s="4"/>
@@ -1961,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I74" s="14">
-        <f t="shared" ref="I74:I76" si="6">G74-H74</f>
+        <f t="shared" ref="I74:I76" si="7">G74-H74</f>
         <v>3</v>
       </c>
       <c r="J74" s="4"/>
@@ -1980,7 +2002,7 @@
         <v>0</v>
       </c>
       <c r="I75" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J75" s="4"/>
@@ -1999,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="I76" s="14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J76" s="4"/>
@@ -2219,7 +2241,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,6 +2306,10 @@
       <c r="F6">
         <v>3</v>
       </c>
+      <c r="H6" s="19"/>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2301,6 +2327,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>32</v>
@@ -2320,6 +2351,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>